<commit_message>
new file:   "data/siheung_real/raw/CODE \354\240\225\354\235\230\354\204\234.xlsx" 	new file:   "data/siheung_real/raw/\352\265\220\354\260\250\353\241\234_\354\240\221\352\267\274\353\241\234 \354\240\225\354\235\230\354\204\234.xlsx" 	new file:   "data/siheung_real/raw/\354\212\244\353\247\210\355\212\270\352\265\220\354\260\250\353\241\234 1\353\266\204 \352\265\220\355\206\265\354\240\225\353\263\264_sample.xlsx" 	modified:   "data/siheung_real/raw/\354\213\234\355\235\245\354\213\234_m_road_crsrd_inf(\353\235\274\354\236\204\354\227\220\354\212\244)_\354\212\244\353\247\210\355\212\270CCTV \353\247\210\354\212\244\355\204\260 \353\215\260\354\235\264\355\204\260_\352\270\260\354\264\210\353\215\260\354\235\264\355\204\260.xlsx"
</commit_message>
<xml_diff>
--- a/data/siheung_real/raw/시흥시_m_road_crsrd_inf(라임에스)_스마트CCTV 마스터 데이터_기초데이터.xlsx
+++ b/data/siheung_real/raw/시흥시_m_road_crsrd_inf(라임에스)_스마트CCTV 마스터 데이터_기초데이터.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\10. 작업폴더\2021_01_19 자율주행 기술개발 혁신사업\40. 작업 폴더\2단계_2차년\9월\시흥TB_스마트교차로 연계관련 자료\시흥시ITS 테이블데이터_20250907\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4122AD58-142F-4A3D-A8A3-2D4B3773A507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15A9A75-B6B2-4DBF-91A8-4DFD94D34C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="63890" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>SH001N0071</t>
   </si>
   <si>
-    <t>SH001N0006</t>
-  </si>
-  <si>
     <t>SH001N0004</t>
   </si>
   <si>
@@ -677,6 +674,10 @@
   </si>
   <si>
     <t>SH009N0002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SH001N0006</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1013,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1036,42 +1037,42 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>90</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>91</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>92</v>
-      </c>
-      <c r="K1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2">
         <v>126.7439866</v>
@@ -1086,7 +1087,7 @@
         <v>6431</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I2" s="1">
         <v>44166</v>
@@ -1094,10 +1095,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3">
         <v>126.7379523</v>
@@ -1112,7 +1113,7 @@
         <v>8981</v>
       </c>
       <c r="H3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I3" s="1">
         <v>44166</v>
@@ -1120,10 +1121,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4">
         <v>126.74789939999999</v>
@@ -1138,7 +1139,7 @@
         <v>7174</v>
       </c>
       <c r="H4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I4" s="1">
         <v>44166</v>
@@ -1146,10 +1147,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5">
         <v>126.7341916</v>
@@ -1164,7 +1165,7 @@
         <v>31671</v>
       </c>
       <c r="H5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I5" s="1">
         <v>44166</v>
@@ -1172,10 +1173,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6">
         <v>126.7806734</v>
@@ -1190,7 +1191,7 @@
         <v>6277</v>
       </c>
       <c r="H6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I6" s="1">
         <v>44166</v>
@@ -1201,10 +1202,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>216</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7">
         <v>126.7217679</v>
@@ -1219,7 +1220,7 @@
         <v>20504</v>
       </c>
       <c r="H7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I7" s="1">
         <v>44166</v>
@@ -1230,10 +1231,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8">
         <v>126.76199509999999</v>
@@ -1248,7 +1249,7 @@
         <v>7775</v>
       </c>
       <c r="H8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I8" s="1">
         <v>44166</v>
@@ -1259,7 +1260,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9">
         <v>126.71533719999999</v>
@@ -1274,7 +1275,7 @@
         <v>14135</v>
       </c>
       <c r="H9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I9" s="1">
         <v>44166</v>
@@ -1282,10 +1283,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10">
         <v>126.7450834</v>
@@ -1300,7 +1301,7 @@
         <v>6401</v>
       </c>
       <c r="H10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I10" s="1">
         <v>44166</v>
@@ -1308,10 +1309,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11">
         <v>126.80883439999999</v>
@@ -1326,7 +1327,7 @@
         <v>9289</v>
       </c>
       <c r="H11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I11" s="1">
         <v>44166</v>
@@ -1334,10 +1335,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12">
         <v>126.78687669999999</v>
@@ -1352,7 +1353,7 @@
         <v>11541</v>
       </c>
       <c r="H12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I12" s="1">
         <v>44166</v>
@@ -1360,10 +1361,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13">
         <v>126.7964702</v>
@@ -1378,7 +1379,7 @@
         <v>4675</v>
       </c>
       <c r="H13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I13" s="1">
         <v>44166</v>
@@ -1386,10 +1387,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14">
         <v>126.7422806</v>
@@ -1404,7 +1405,7 @@
         <v>6567</v>
       </c>
       <c r="H14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I14" s="1">
         <v>44166</v>
@@ -1412,10 +1413,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15">
         <v>126.8617354</v>
@@ -1430,7 +1431,7 @@
         <v>10084</v>
       </c>
       <c r="H15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I15" s="1">
         <v>44166</v>
@@ -1438,10 +1439,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16">
         <v>126.86748780000001</v>
@@ -1456,7 +1457,7 @@
         <v>14952</v>
       </c>
       <c r="H16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I16" s="1">
         <v>44166</v>
@@ -1464,10 +1465,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17">
         <v>126.8296569</v>
@@ -1482,7 +1483,7 @@
         <v>10530</v>
       </c>
       <c r="H17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I17" s="1">
         <v>44166</v>
@@ -1490,10 +1491,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18">
         <v>126.7416903</v>
@@ -1508,7 +1509,7 @@
         <v>6926</v>
       </c>
       <c r="H18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I18" s="1">
         <v>44166</v>
@@ -1516,10 +1517,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19">
         <v>126.734737</v>
@@ -1534,7 +1535,7 @@
         <v>7714</v>
       </c>
       <c r="H19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I19" s="1">
         <v>44166</v>
@@ -1542,10 +1543,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C20">
         <v>126.73331810000001</v>
@@ -1560,7 +1561,7 @@
         <v>7322</v>
       </c>
       <c r="H20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I20" s="1">
         <v>44166</v>
@@ -1568,10 +1569,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C21">
         <v>126.7407199</v>
@@ -1586,7 +1587,7 @@
         <v>7507</v>
       </c>
       <c r="H21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I21" s="1">
         <v>44166</v>
@@ -1594,10 +1595,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C22">
         <v>126.73934819999999</v>
@@ -1612,7 +1613,7 @@
         <v>13497</v>
       </c>
       <c r="H22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I22" s="1">
         <v>44166</v>
@@ -1620,10 +1621,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C23">
         <v>126.7363491</v>
@@ -1638,7 +1639,7 @@
         <v>19678</v>
       </c>
       <c r="H23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I23" s="1">
         <v>44166</v>
@@ -1646,10 +1647,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24">
         <v>126.7420223</v>
@@ -1664,7 +1665,7 @@
         <v>16588</v>
       </c>
       <c r="H24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I24" s="1">
         <v>44166</v>
@@ -1672,10 +1673,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25">
         <v>126.7477327</v>
@@ -1690,7 +1691,7 @@
         <v>13388</v>
       </c>
       <c r="H25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I25" s="1">
         <v>44166</v>
@@ -1698,10 +1699,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26">
         <v>126.75304610000001</v>
@@ -1716,7 +1717,7 @@
         <v>16302</v>
       </c>
       <c r="H26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I26" s="1">
         <v>44166</v>
@@ -1724,10 +1725,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C27">
         <v>126.7507895</v>
@@ -1742,7 +1743,7 @@
         <v>9201</v>
       </c>
       <c r="H27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I27" s="1">
         <v>44166</v>
@@ -1750,10 +1751,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28">
         <v>126.75608219999999</v>
@@ -1768,7 +1769,7 @@
         <v>6814</v>
       </c>
       <c r="H28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I28" s="1">
         <v>44166</v>
@@ -1779,7 +1780,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29">
         <v>126.7919351</v>
@@ -1794,7 +1795,7 @@
         <v>11493</v>
       </c>
       <c r="H29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J29" s="1">
         <v>44690.616168981483</v>
@@ -1802,10 +1803,10 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" t="s">
         <v>123</v>
-      </c>
-      <c r="B30" t="s">
-        <v>124</v>
       </c>
       <c r="C30">
         <v>126.77382</v>
@@ -1817,15 +1818,15 @@
         <v>101</v>
       </c>
       <c r="H30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" t="s">
         <v>126</v>
-      </c>
-      <c r="B31" t="s">
-        <v>127</v>
       </c>
       <c r="C31">
         <v>126.84675300000001</v>
@@ -1837,15 +1838,15 @@
         <v>101</v>
       </c>
       <c r="H31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" t="s">
         <v>128</v>
-      </c>
-      <c r="B32" t="s">
-        <v>129</v>
       </c>
       <c r="C32">
         <v>126.75007100000001</v>
@@ -1857,15 +1858,15 @@
         <v>101</v>
       </c>
       <c r="H32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" t="s">
         <v>130</v>
-      </c>
-      <c r="B33" t="s">
-        <v>131</v>
       </c>
       <c r="C33">
         <v>126.73554300000001</v>
@@ -1877,15 +1878,15 @@
         <v>101</v>
       </c>
       <c r="H33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C34">
         <v>126.692328</v>
@@ -1900,15 +1901,15 @@
         <v>2953</v>
       </c>
       <c r="H34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" t="s">
         <v>133</v>
-      </c>
-      <c r="B35" t="s">
-        <v>134</v>
       </c>
       <c r="C35">
         <v>126.788622</v>
@@ -1920,15 +1921,15 @@
         <v>101</v>
       </c>
       <c r="H35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" t="s">
         <v>135</v>
-      </c>
-      <c r="B36" t="s">
-        <v>136</v>
       </c>
       <c r="C36">
         <v>126.704504</v>
@@ -1940,15 +1941,15 @@
         <v>101</v>
       </c>
       <c r="H36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" t="s">
         <v>137</v>
-      </c>
-      <c r="B37" t="s">
-        <v>138</v>
       </c>
       <c r="C37">
         <v>126.709867</v>
@@ -1960,15 +1961,15 @@
         <v>101</v>
       </c>
       <c r="H37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" t="s">
         <v>139</v>
-      </c>
-      <c r="B38" t="s">
-        <v>140</v>
       </c>
       <c r="C38">
         <v>127.07541500000001</v>
@@ -1980,15 +1981,15 @@
         <v>101</v>
       </c>
       <c r="H38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" t="s">
         <v>141</v>
-      </c>
-      <c r="B39" t="s">
-        <v>142</v>
       </c>
       <c r="C39">
         <v>126.723212</v>
@@ -2000,15 +2001,15 @@
         <v>101</v>
       </c>
       <c r="H39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" t="s">
         <v>143</v>
-      </c>
-      <c r="B40" t="s">
-        <v>144</v>
       </c>
       <c r="C40">
         <v>126.72668899999999</v>
@@ -2020,15 +2021,15 @@
         <v>101</v>
       </c>
       <c r="H40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
+        <v>144</v>
+      </c>
+      <c r="B41" t="s">
         <v>145</v>
-      </c>
-      <c r="B41" t="s">
-        <v>146</v>
       </c>
       <c r="C41">
         <v>126.71608000000001</v>
@@ -2040,15 +2041,15 @@
         <v>101</v>
       </c>
       <c r="H41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" t="s">
         <v>147</v>
-      </c>
-      <c r="B42" t="s">
-        <v>148</v>
       </c>
       <c r="C42">
         <v>126.834541</v>
@@ -2060,15 +2061,15 @@
         <v>101</v>
       </c>
       <c r="H42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
+        <v>148</v>
+      </c>
+      <c r="B43" t="s">
         <v>149</v>
-      </c>
-      <c r="B43" t="s">
-        <v>150</v>
       </c>
       <c r="C43">
         <v>126.730605</v>
@@ -2080,15 +2081,15 @@
         <v>101</v>
       </c>
       <c r="H43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
+        <v>150</v>
+      </c>
+      <c r="B44" t="s">
         <v>151</v>
-      </c>
-      <c r="B44" t="s">
-        <v>152</v>
       </c>
       <c r="C44">
         <v>126.866281</v>
@@ -2100,15 +2101,15 @@
         <v>101</v>
       </c>
       <c r="H44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C45">
         <v>126.76613999999999</v>
@@ -2123,7 +2124,7 @@
         <v>9380</v>
       </c>
       <c r="H45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.45">
@@ -2131,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C46">
         <v>126.80270470000001</v>
@@ -2146,7 +2147,7 @@
         <v>26476</v>
       </c>
       <c r="H46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J46" s="1">
         <v>44690.455462962964</v>
@@ -2157,7 +2158,7 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C47">
         <v>126.790511</v>
@@ -2172,7 +2173,7 @@
         <v>11492</v>
       </c>
       <c r="H47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.45">
@@ -2180,7 +2181,7 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C48">
         <v>126.786345</v>
@@ -2195,15 +2196,15 @@
         <v>9481</v>
       </c>
       <c r="H48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C49">
         <v>126.788849</v>
@@ -2218,7 +2219,7 @@
         <v>7159</v>
       </c>
       <c r="H49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.45">
@@ -2226,7 +2227,7 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C50">
         <v>126.773948</v>
@@ -2241,15 +2242,15 @@
         <v>10832</v>
       </c>
       <c r="H50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C51">
         <v>126.772515</v>
@@ -2264,15 +2265,15 @@
         <v>6650</v>
       </c>
       <c r="H51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C52">
         <v>126.792635</v>
@@ -2287,15 +2288,15 @@
         <v>13677</v>
       </c>
       <c r="H52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C53">
         <v>126.852616</v>
@@ -2310,15 +2311,15 @@
         <v>7318</v>
       </c>
       <c r="H53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C54">
         <v>126.821378</v>
@@ -2333,15 +2334,15 @@
         <v>10302</v>
       </c>
       <c r="H54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C55">
         <v>126.81697200000001</v>
@@ -2356,7 +2357,7 @@
         <v>6801</v>
       </c>
       <c r="H55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.45">
@@ -2364,7 +2365,7 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C56">
         <v>126.706563</v>
@@ -2379,7 +2380,7 @@
         <v>13901</v>
       </c>
       <c r="H56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.45">
@@ -2387,7 +2388,7 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C57">
         <v>126.744866</v>
@@ -2402,7 +2403,7 @@
         <v>18709</v>
       </c>
       <c r="H57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.45">
@@ -2410,7 +2411,7 @@
         <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C58">
         <v>126.74803199999999</v>
@@ -2425,15 +2426,15 @@
         <v>19068</v>
       </c>
       <c r="H58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C59">
         <v>126.720755</v>
@@ -2448,15 +2449,15 @@
         <v>10676</v>
       </c>
       <c r="H59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C60">
         <v>126.723096</v>
@@ -2471,15 +2472,15 @@
         <v>10548</v>
       </c>
       <c r="H60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C61">
         <v>126.726331</v>
@@ -2494,7 +2495,7 @@
         <v>12701</v>
       </c>
       <c r="H61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K61">
         <v>168</v>
@@ -2502,10 +2503,10 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C62">
         <v>126.72865899999999</v>
@@ -2520,15 +2521,15 @@
         <v>11610</v>
       </c>
       <c r="H62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C63">
         <v>126.73111400000001</v>
@@ -2543,15 +2544,15 @@
         <v>6253</v>
       </c>
       <c r="H63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C64">
         <v>126.733501</v>
@@ -2566,15 +2567,15 @@
         <v>7896</v>
       </c>
       <c r="H64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C65">
         <v>126.731207</v>
@@ -2589,15 +2590,15 @@
         <v>9193</v>
       </c>
       <c r="H65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C66">
         <v>126.729046</v>
@@ -2612,15 +2613,15 @@
         <v>7600</v>
       </c>
       <c r="H66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C67">
         <v>126.72718</v>
@@ -2635,15 +2636,15 @@
         <v>9294</v>
       </c>
       <c r="H67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C68">
         <v>126.730615</v>
@@ -2658,15 +2659,15 @@
         <v>4276</v>
       </c>
       <c r="H68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C69">
         <v>126.79306200000001</v>
@@ -2681,7 +2682,7 @@
         <v>6436</v>
       </c>
       <c r="H69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I69" s="1">
         <v>45035.483217592591</v>
@@ -2689,10 +2690,10 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B70" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C70">
         <v>126.8044793</v>
@@ -2707,7 +2708,7 @@
         <v>12639</v>
       </c>
       <c r="H70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I70" s="1">
         <v>45035.483217592591</v>
@@ -2715,10 +2716,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C71">
         <v>126.80743</v>
@@ -2733,7 +2734,7 @@
         <v>12990</v>
       </c>
       <c r="H71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I71" s="1">
         <v>45035.483217592591</v>
@@ -2741,10 +2742,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B72" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C72">
         <v>126.82261</v>
@@ -2759,7 +2760,7 @@
         <v>6676</v>
       </c>
       <c r="H72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I72" s="1">
         <v>45035.483217592591</v>
@@ -2767,10 +2768,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B73" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C73">
         <v>126.7920383</v>
@@ -2785,7 +2786,7 @@
         <v>4470</v>
       </c>
       <c r="H73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I73" s="1">
         <v>45035.483217592591</v>
@@ -2793,10 +2794,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B74" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C74">
         <v>126.78946860000001</v>
@@ -2811,7 +2812,7 @@
         <v>5323</v>
       </c>
       <c r="H74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I74" s="1">
         <v>45035.483217592591</v>
@@ -2819,10 +2820,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B75" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C75">
         <v>126.79597149999999</v>
@@ -2837,7 +2838,7 @@
         <v>17461</v>
       </c>
       <c r="H75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I75" s="1">
         <v>45035.483217592591</v>
@@ -2845,10 +2846,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B76" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C76">
         <v>126.71775599999999</v>
@@ -2863,7 +2864,7 @@
         <v>3511</v>
       </c>
       <c r="H76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I76" s="1">
         <v>45035.483217592591</v>
@@ -2871,10 +2872,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B77" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C77">
         <v>126.723305</v>
@@ -2889,7 +2890,7 @@
         <v>6256</v>
       </c>
       <c r="H77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I77" s="1">
         <v>45035.483217592591</v>
@@ -2897,10 +2898,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B78" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C78">
         <v>126.725694</v>
@@ -2915,7 +2916,7 @@
         <v>3354</v>
       </c>
       <c r="H78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I78" s="1">
         <v>45035.483217592591</v>
@@ -2923,10 +2924,10 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C79">
         <v>126.728104</v>
@@ -2941,7 +2942,7 @@
         <v>4011</v>
       </c>
       <c r="H79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I79" s="1">
         <v>45035.483217592591</v>
@@ -2949,10 +2950,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C80">
         <v>126.730476</v>
@@ -2967,7 +2968,7 @@
         <v>3249</v>
       </c>
       <c r="H80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I80" s="1">
         <v>45035.483217592591</v>
@@ -2975,10 +2976,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B81" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C81">
         <v>126.73620699999999</v>
@@ -2993,7 +2994,7 @@
         <v>3150</v>
       </c>
       <c r="H81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I81" s="1">
         <v>45035.483217592591</v>
@@ -3001,10 +3002,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B82" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C82">
         <v>126.73901499999999</v>
@@ -3019,7 +3020,7 @@
         <v>3385</v>
       </c>
       <c r="H82" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I82" s="1">
         <v>45035.483217592591</v>
@@ -3027,10 +3028,10 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B83" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C83">
         <v>126.73944400000001</v>
@@ -3045,7 +3046,7 @@
         <v>6383</v>
       </c>
       <c r="H83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I83" s="1">
         <v>45035.483217592591</v>
@@ -3053,10 +3054,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B84" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C84">
         <v>126.737799</v>
@@ -3071,7 +3072,7 @@
         <v>4525</v>
       </c>
       <c r="H84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I84" s="1">
         <v>45035.483217592591</v>
@@ -3079,10 +3080,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B85" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C85">
         <v>126.746994</v>
@@ -3097,7 +3098,7 @@
         <v>2511</v>
       </c>
       <c r="H85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I85" s="1">
         <v>45035.483217592591</v>
@@ -3105,10 +3106,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B86" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C86">
         <v>126.75017</v>
@@ -3123,7 +3124,7 @@
         <v>1906</v>
       </c>
       <c r="H86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I86" s="1">
         <v>45035.483217592591</v>
@@ -3131,10 +3132,10 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B87" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C87">
         <v>126.75491</v>
@@ -3149,7 +3150,7 @@
         <v>2506</v>
       </c>
       <c r="H87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I87" s="1">
         <v>45035.483217592591</v>
@@ -3157,10 +3158,10 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B88" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C88">
         <v>126.758506</v>
@@ -3175,7 +3176,7 @@
         <v>3192</v>
       </c>
       <c r="H88" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I88" s="1">
         <v>45035.483217592591</v>
@@ -3183,10 +3184,10 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B89" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C89">
         <v>126.75727999999999</v>
@@ -3201,7 +3202,7 @@
         <v>3450</v>
       </c>
       <c r="H89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I89" s="1">
         <v>45035.483217592591</v>
@@ -3212,7 +3213,7 @@
         <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C90">
         <v>126.77379500000001</v>
@@ -3227,7 +3228,7 @@
         <v>9624</v>
       </c>
       <c r="H90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I90" s="1">
         <v>45035.483217592591</v>
@@ -3235,10 +3236,10 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B91" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C91">
         <v>126.846782</v>
@@ -3253,7 +3254,7 @@
         <v>12488</v>
       </c>
       <c r="H91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I91" s="1">
         <v>45035.483217592591</v>
@@ -3261,10 +3262,10 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B92" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C92">
         <v>126.72013699999999</v>
@@ -3279,7 +3280,7 @@
         <v>2885</v>
       </c>
       <c r="H92" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I92" s="1">
         <v>45035.483217592591</v>
@@ -3287,10 +3288,10 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B93" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C93">
         <v>126.736355</v>
@@ -3305,7 +3306,7 @@
         <v>4556</v>
       </c>
       <c r="H93" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I93" s="1">
         <v>45035.483217592591</v>
@@ -3313,10 +3314,10 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B94" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C94">
         <v>126.744057</v>
@@ -3331,7 +3332,7 @@
         <v>4094</v>
       </c>
       <c r="H94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I94" s="1">
         <v>45035.483217592591</v>
@@ -3342,7 +3343,7 @@
         <v>7</v>
       </c>
       <c r="B95" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C95">
         <v>126.750146</v>
@@ -3357,7 +3358,7 @@
         <v>15564</v>
       </c>
       <c r="H95" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I95" s="1">
         <v>45035.483217592591</v>
@@ -3365,10 +3366,10 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B96" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C96">
         <v>126.773989</v>
@@ -3383,7 +3384,7 @@
         <v>5685</v>
       </c>
       <c r="H96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I96" s="1">
         <v>45035.483217592591</v>
@@ -3391,10 +3392,10 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B97" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C97">
         <v>126.7645946</v>
@@ -3409,7 +3410,7 @@
         <v>3912</v>
       </c>
       <c r="H97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I97" s="1">
         <v>45035.483217592591</v>
@@ -3417,10 +3418,10 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C98">
         <v>126.74472900000001</v>
@@ -3435,7 +3436,7 @@
         <v>6019</v>
       </c>
       <c r="H98" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I98" s="1">
         <v>45035.483217592591</v>
@@ -3443,10 +3444,10 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C99" s="2">
         <v>126.72803740000001</v>
@@ -3462,7 +3463,7 @@
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I99" s="3">
         <v>45796.741168981483</v>
@@ -3476,10 +3477,10 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A100" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C100" s="2">
         <v>126.72938670000001</v>
@@ -3495,7 +3496,7 @@
       </c>
       <c r="G100" s="2"/>
       <c r="H100" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I100" s="3">
         <v>45796.741168981483</v>
@@ -3509,10 +3510,10 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="C101" s="2">
         <v>126.7262075</v>
@@ -3528,7 +3529,7 @@
       </c>
       <c r="G101" s="2"/>
       <c r="H101" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I101" s="3">
         <v>45796.741168981483</v>
@@ -3542,10 +3543,10 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="C102" s="2">
         <v>126.7322391</v>
@@ -3561,7 +3562,7 @@
       </c>
       <c r="G102" s="2"/>
       <c r="H102" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I102" s="3">
         <v>45796.741168981483</v>
@@ -3575,10 +3576,10 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="C103" s="2">
         <v>126.73102729999999</v>
@@ -3594,7 +3595,7 @@
       </c>
       <c r="G103" s="2"/>
       <c r="H103" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I103" s="3">
         <v>45796.741168981483</v>

</xml_diff>